<commit_message>
use php file instant of html, add inventory form , change table style, change css.
</commit_message>
<xml_diff>
--- a/ratana/Expenditure/expenditure cycle.xlsx
+++ b/ratana/Expenditure/expenditure cycle.xlsx
@@ -125,10 +125,10 @@
     <t>TEL.</t>
   </si>
   <si>
-    <t>product</t>
-  </si>
-  <si>
     <t>(receive invoice from vender?)</t>
+  </si>
+  <si>
+    <t>product(What product? Or different vendor has different product?)</t>
   </si>
 </sst>
 </file>
@@ -179,10 +179,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,7 +501,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25:F26"/>
+      <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -524,95 +525,116 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F12" t="s">
-        <v>31</v>
-      </c>
+      <c r="F12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -665,56 +687,64 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="A21" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="A22" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F22" t="s">
+      <c r="F22" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C25" s="2"/>
+      <c r="B25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="A26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E26" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="1" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>